<commit_message>
Check in on 8/20 to run full suite
</commit_message>
<xml_diff>
--- a/TestDataAndResults/TestData/RealTimeAutoAPI.xlsx
+++ b/TestDataAndResults/TestData/RealTimeAutoAPI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\SofieKDF_HeadLess_5819_V2\SofieKDF_HeadLess_5819\SofieKDFHeadless\TestDataAndResults\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB142C2-7770-495F-8C4F-973B910C5CBE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A253D32B-7145-4E03-AB7A-3380FEE374E3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RealtimeSpineData" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
   <si>
     <t>SpineType</t>
   </si>
@@ -43,63 +43,43 @@
     <t>DBTable</t>
   </si>
   <si>
-    <t>{"pxObjClass":"ADQURA-FW-AppsFW-Data-PartyStaging","provider_type":"Doctor","country":"US","specialty":"International","city":"Doral","first_order_date":"20020501T070000.000 GMT","provider_closed":0,"location_id":8631,"do_not_mail":1,"record_ts":"20181113T023246.000 GMT","billingaccount_id":"10-177702","state":"FL","lab_id":10,"first_name":"JXXn","zipcode1":"33122","lifetime_percent_cases_wi24L":"0.12","deleted_flg":"N","address2":"SXXXXXXXX4","provider_email":"1261384919@test.glidewell.com","address1":"2XXXXXXXXXXXXXXe","last_name":"SXXXXXXXXXXX.","current_sales_stage":"Committed","snapshot_uid":10072,"lifetime_remake_percent":0.19,"full_name":"JXXn SXXXXXXXXXXX.","most_recent_order_date":"20181109T223300.000 GMT","provider_status":"Active","specialty_id":"INT","do_not_email":0,"party_id":"1016267_8631_10","provider_id":1016267,"cod":0,"locationtype":"Shipping","salutation":"Dr. SXXXXXXXXXXX."}</t>
-  </si>
-  <si>
-    <t>{"pxObjClass":"ADQURA-FW-AppsFW-Data-PartyStaging","provider_type":"Doctor","country":"US","city":"Vallejo","first_order_date":"20170814T175200.000 GMT","provider_closed":0,"location_id":3783,"do_not_mail":1,"record_ts":"20181113T023246.000 GMT","billingaccount_id":"10-1569852","state":"CA","lab_id":10,"first_name":"CXXXXXXn","zipcode1":"94590","lifetime_percent_cases_wi24L":"0.02","deleted_flg":"N","address2":"SXXXA","provider_email":"1340482834@test.glidewell.com","address1":"2XXXXXXXXXXXXXt","last_name":"CXXi","current_sales_stage":"Non-Committed","snapshot_uid":10073,"lifetime_remake_percent":0.34,"full_name":"CXXXXXXn CXXi","most_recent_order_date":"20180908T001800.000 GMT","provider_status":"Active","specialty_id":"GND","do_not_email":0,"party_id":"1016286_3783_10","provider_id":1016286,"cod":0,"locationtype":"Shipping","salutation":"Dr. CXXi"}</t>
-  </si>
-  <si>
-    <t>{"pxObjClass":"ADQURA-FW-AppsFW-Data-PartyStaging","provider_type":"Doctor","country":"US","specialty":"General Dentist","city":"Fort Worth","first_order_date":"19990608T070000.000 GMT","provider_closed":0,"location_id":8906,"do_not_mail":0,"restart_date":"20031113T080000.000 GMT","record_ts":"20181113T023246.000 GMT","billingaccount_id":"10-157685","state":"TX","lab_id":10,"first_name":"SXXXXXn","zipcode1":"76109","lifetime_percent_cases_wi24L":"0.14","deleted_flg":"N","address2":"SXXXXX4","provider_email":"2670007766@test.glidewell.com","address1":"3XXXXXXXXXXXXXXd","last_name":"BXXXXXn","current_sales_stage":"Non-Committed","snapshot_uid":10074,"lifetime_remake_percent":0.12,"full_name":"SXXXXXn BXXXXXn","most_recent_order_date":"20181108T233400.000 GMT","provider_status":"Active","specialty_id":"GND","do_not_email":0,"party_id":"1016361_8906_10","provider_id":1016361,"cod":0,"locationtype":"Shipping","salutation":"Dr. BXXXXXn"}</t>
-  </si>
-  <si>
     <t>ADQURA-FW-AppsFW-Data-AgreementStaging</t>
   </si>
   <si>
-    <t>{"AgreementType":"Postpay","AgreementID":"A123832","BillingAddressID":"21052791","RecordTS":"20160520T000000.000 GMT","AgreementCategory":"Mobile","BillingAddressLine1":"0/1","AccountStatus":"Active","BillingAddressLine2":"24 Ballantay Road","BillingAddressLine3":"GLASGOW","PartyID":"﻿123832","AgreementEndDate":"20190417T000000.000 GMT","AccountStartDate":"20160520T000000.000 GMT","AccountPaymentType":"DirectDebit","AgreementStatus":"Active","AccountEndDate":"20170520T000000.000 GMT","AccountID":"ACC123832","BillingCycleDay":"21","AccountType":"Consumer","AgreementStartDate":"20180929T000000.000 GMT","AgreementPartyRoles":"Subscriber","DeletedFlag":"N","BillingAddressCountry":"UK","BillingAddressPostcode":"G45 0EA","BillingAddressVLDFlag":"Y"}</t>
-  </si>
-  <si>
-    <t>{"AgreementType":"Postpay","AgreementID":"A123833","BillingAddressID":"15017484","RecordTS":"20170423T000000.000 GMT","AgreementCategory":"Mobile","BillingAddressLine1":"16 MILBOURN COURT","AccountStatus":"Active","BillingAddressLine2":"MIDDLE MEAD","BillingAddressLine3":"ROCHFORD","PartyID":"123833","AgreementEndDate":"20190417T000000.000 GMT","AccountStartDate":"20090308T000000.000 GMT","AccountPaymentType":"DirectDebit","AgreementStatus":"Active","AccountEndDate":"20180423T000000.000 GMT","AccountID":"ACC123833","BillingCycleDay":"10","AccountType":"Consumer","AgreementStartDate":"20180929T000000.000 GMT","AgreementPartyRoles":"Decision Maker","DeletedFlag":"N","BillingAddressCountry":"UK","BillingAddressPostcode":"SS4 1UY","BillingAddressVLDFlag":"Y"}</t>
-  </si>
-  <si>
-    <t>{"AgreementType":"Postpay","AccountEndDate":"20171025T000000.000 GMT","AgreementID":"A123834","AccountID":"ACC123834","BillingAddressID":"9087722","BillingCycleDay":"9","RecordTS":"20161025T000000.000 GMT","AgreementCategory":"Mobile","AccountType":"Consumer","BillingAddressLine1":"24 Farm Walk","AccountStatus":"Active","BillingAddressLine2":"ROCHDALE","AgreementStartDate":"20180929T000000.000 GMT","PartyID":"123834","AgreementEndDate":"20190417T000000.000 GMT","AccountStartDate":"20070315T000000.000 GMT","AgreementPartyRoles":"Decision Maker","DeletedFlag":"N","AccountPaymentType":"DirectDebit","BillingAddressCountry":"UK","AgreementStatus":"Active","BillingAddressPostcode":"OL16 2TN","BillingAddressVLDFlag":"Y"}</t>
-  </si>
-  <si>
     <t>ADQURA-FW-AppsFW-Data-EventStaging</t>
   </si>
   <si>
-    <t>{"event_id":"143812708167417769751178198894049310955","event_type":"bill_created","deleted_flg":"N","record_ts":"20180514T212752.000 GMT","event_ts":"20180514T212752.000 GMT","party_id":"123489","context":"account_id=ACC123489,bill_no=AAP99577821,bill_period_start_ts=20180514 21:27:52,bill_period_end_ts=20180613 21:27:52,bill_amt=57,bill_bal_amt=0,first_bill_flg=Y","entity_id":"A123489"}</t>
-  </si>
-  <si>
-    <t>{"event_id":"143812708167418978676997813523224017131","event_type":"bill_created","deleted_flg":"N","record_ts":"20180514T212752.000 GMT","event_ts":"20180514T212752.000 GMT","party_id":"123490","context":"account_id=ACC123490,bill_no=AAP1690569,bill_period_start_ts=20180514 21:27:52,bill_period_end_ts=20180613 21:27:52,bill_amt=70,bill_bal_amt=0,first_bill_flg=Y","entity_id":"A123490"}</t>
-  </si>
-  <si>
-    <t>{"event_id":"143812708167421396528637042781573429483","event_type":"bill_created","deleted_flg":"N","record_ts":"20180514T212752.000 GMT","event_ts":"20180514T212752.000 GMT","party_id":"123492","context":"account_id=ACC123492,bill_no=AAP30568656,bill_period_start_ts=20180514 21:27:52,bill_period_end_ts=20180613 21:27:52,bill_amt=38,bill_bal_amt=0,first_bill_flg=Y","entity_id":"A123492"}</t>
-  </si>
-  <si>
-    <t>{"AgreementType":"Postpay","AgreementID":"A123832","BillingAddressID":"21052791","RecordTS":"20160520T000000.000 GMT","AgreementCategory":"Mobile","BillingAddressLine1":"0/1","AccountStatus":"Active","BillingAddressLine2":"24 Ballantay Road","BillingAddressLine3":"GLASGOW","PartyID":"﻿123832","AgreementEndDate":"20190417T000000.000 GMT","AccountStartDate":"20160520T000000.000 GMT","AccountPaymentType":"DirectDebit","AgreementStatus":"Active","AccountEndDate":"20170520T000000.000 GMT","AccountID":"ACC123832","BillingCycleDay":"21","AccountType":"Consumer","AgreementStartDate":"20180929T000000.000 GMT","AgreementPartyRoles":"Subscriber","DeletedFlag":"N","BillingAddressCountry":"UK","BillingAddressPostcode":"G45 0EA","BillingAddressVLDFlag":"Y","NewTestProperty":"autoTest1"}</t>
-  </si>
-  <si>
-    <t>{"AgreementType":"Postpay","AgreementID":"A123833","BillingAddressID":"15017484","RecordTS":"20170423T000000.000 GMT","AgreementCategory":"Mobile","BillingAddressLine1":"16 MILBOURN COURT","AccountStatus":"Active","BillingAddressLine2":"MIDDLE MEAD","BillingAddressLine3":"ROCHFORD","PartyID":"123833","AgreementEndDate":"20190417T000000.000 GMT","AccountStartDate":"20090308T000000.000 GMT","AccountPaymentType":"DirectDebit","AgreementStatus":"Active","AccountEndDate":"20180423T000000.000 GMT","AccountID":"ACC123833","BillingCycleDay":"10","AccountType":"Consumer","AgreementStartDate":"20180929T000000.000 GMT","AgreementPartyRoles":"Decision Maker","DeletedFlag":"N","BillingAddressCountry":"UK","BillingAddressPostcode":"SS4 1UY","BillingAddressVLDFlag":"Y","NewTestProperty":"autoTest2"}</t>
-  </si>
-  <si>
-    <t>{"AgreementType":"Postpay","AccountEndDate":"20171025T000000.000 GMT","AgreementID":"A123834","AccountID":"ACC123834","BillingAddressID":"9087722","BillingCycleDay":"9","RecordTS":"20161025T000000.000 GMT","AgreementCategory":"Mobile","AccountType":"Consumer","BillingAddressLine1":"24 Farm Walk","AccountStatus":"Active","BillingAddressLine2":"ROCHDALE","AgreementStartDate":"20180929T000000.000 GMT","PartyID":"123834","AgreementEndDate":"20190417T000000.000 GMT","AccountStartDate":"20070315T000000.000 GMT","AgreementPartyRoles":"Decision Maker","DeletedFlag":"N","AccountPaymentType":"DirectDebit","BillingAddressCountry":"UK","AgreementStatus":"Active","BillingAddressPostcode":"OL16 2TN","BillingAddressVLDFlag":"Y","NewTestProperty":"autoTest3"}</t>
+    <t>{"AgreementType":"Postpay","AccountEndDate":"20180906T000000.000 GMT","AgreementID":"A124206","AccountID":"ACC124206","BillingAddressID":"6783864","BillingCycleDay":"11","RecordTS":"20170906T000000.000 GMT","AgreementCategory":"Mobile","AccountType":"Consumer","BillingAddressLine1":"33 GOWER ROAD","AccountStatus":"Active","BillingAddressLine2":"STOCKPORT","AgreementStartDate":"20170906T000000.000 GMT","PartyID":"﻿124206","AgreementEndDate":"20190816T000000.000 GMT","AccountStartDate":"20170906T000000.000 GMT","AgreementPartyRoles":"Subscriber","DeletedFlag":"N","AccountPaymentType":"DirectDebit","BillingAddressCountry":"UK","AgreementStatus":"Active","BillingAddressPostcode":"SK4 2QY","BillingAddressVLDFlag":"Y"}</t>
+  </si>
+  <si>
+    <t>{"SegmentKey":"1","ConsentLandline":"Y","LoyaltyJoinTimestamp":"20111209T000000.000 GMT","pyFullName":"Julio Goddard","ConsentMMS":"Y","CustomerID":"123866","Gender":"M","CRMID":"CRM123866","ConsentSMS":"Y","ConsentPersonalData":"Y","DWHID":"DWH123866","RecordTimestamp":"20180313T111357.000 GMT","ConsentLoyalty":"Y","ConsentLetter":"Y","RandomKey":"1","pyCountry":"UK","AddressCount":"1","FirstName":"Julio","ConsentMarketing":"Y","Title":"Mr","ConsentEmail":"Y","ConsentMobile":"Y","ContactTelephoneNumber":"00000457199","CustomerType":"I","Nationality":"British","pyMobilePhone":"10000346088","SMSEligibleFlag":"Y","LoyaltyID":"CLUB123866","LegacyID":"LEG123866","CustomerStatus":"C","DeletedFlag":"N","ContactAddressLine1":"2 OBAN STREET","PartitionKey":"1","ContactAddressID":"3621092","EmailEligibleFlag":"Y","LastName":"Goddard","ContactAddressPostcode":"LS12 3JX","ContactAddressLine2":"LEEDS","ContactAddressVLDFlag":"Y","OnlineID":"DIG123866","pyEmail1":"Julio.Goddard@test.adqura.com","BirthDate":"19850728T000000.000 GMT"}</t>
+  </si>
+  <si>
+    <t>ADQURA-FW-AppsFW-Data-PremiseStaging</t>
+  </si>
+  <si>
+    <t>{"premise_id":"P123456","premise_address_country":"UK","deleted_flg":"N","premise_ownership":"Homeowner","premise_address_line_2":"MILLTIMBER","premise_address_id":"19238471","agreement_id":"A123456","premise_address_line_1":"36 COLTHILL ROAD","record_ts":"20180309T113513.000 GMT","premise_type":"Shared","premise_address_vld_flg":"Y","party_id":"123456","premise_address_postcode":"AB13 0EF"}</t>
+  </si>
+  <si>
+    <t>{"Context":"account_id=ACC124398,bill_no=AAP61363409,bill_period_start_ts=20180514 21:27:52,bill_period_end_ts=20180613 21:27:52,bill_amt=49,bill_bal_amt=0,first_bill_flg=Y","EntityID":"A124398","EntityType":"Prepay","PartyID":"124398","EventType":"bill_created","EventTimestamp":"20180514T212752.000 GMT","RecordTimestamp":"20180514T212752.000 GMT","DeletedFlag":"N","EventID":"﻿143812708168381283629411058346290133227"}</t>
+  </si>
+  <si>
+    <t>ADQURA-FW-AppsFW-Data-ProductStaging</t>
+  </si>
+  <si>
+    <t>{"AgreementID":"A123456","ProductEndDate":"20180611T000000.000 GMT","ProductName":"Bluetooth Headset","ProductType":"Add-On","ProductID":"BLH","ProductStartDate":"20170611T000000.000 GMT","ProductBrand":"Apple","PartyID":"﻿123456","MonthlyCost":"0","RecordTimestamp":"20180313T105548.000 GMT","ProductCategory":"Headset","DeletedFlag":"N","UpfrontCost":"100"}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,9 +102,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -465,102 +444,58 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -575,13 +510,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A719BBE9-0F52-43CD-8A2E-7FC7B9B48DFC}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="45" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -596,35 +536,57 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>